<commit_message>
Excel file improvement Done
</commit_message>
<xml_diff>
--- a/public/sample-format/categories-sync-with-product.xlsx
+++ b/public/sample-format/categories-sync-with-product.xlsx
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t xml:space="preserve">Product Code</t>
+    <t xml:space="preserve">Code</t>
   </si>
   <si>
-    <t xml:space="preserve">Slug</t>
+    <t xml:space="preserve">Slugs</t>
   </si>
   <si>
     <t xml:space="preserve">TAGTEST</t>
@@ -47,7 +47,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -84,12 +84,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -140,7 +134,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -150,10 +144,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -237,10 +227,10 @@
   <dimension ref="A1:AH848"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.51171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.51953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.29"/>
@@ -316,7 +306,7 @@
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2"/>

</xml_diff>